<commit_message>
add data to tmc template
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Recharges_Performer_TMC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF9DB44-0B14-414E-8E1F-207BBCD13729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7E769D-303E-43BB-995D-63CF97C53CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -178,9 +178,6 @@
     <t>InvoiceSummarySheetName</t>
   </si>
   <si>
-    <t>VodafoneActiveListSheetName</t>
-  </si>
-  <si>
     <t>active list</t>
   </si>
   <si>
@@ -232,12 +229,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>VodafoneActiveListRange</t>
-  </si>
-  <si>
-    <t>VodafoneActiveListReadRange</t>
-  </si>
-  <si>
     <t>A2:K9999</t>
   </si>
   <si>
@@ -280,21 +271,6 @@
     <t>vbaCopyColumnDataInRange</t>
   </si>
   <si>
-    <t>VodafoneWorkingsSheetName</t>
-  </si>
-  <si>
-    <t>Workings</t>
-  </si>
-  <si>
-    <t>VodafonePivotByCCSheetName</t>
-  </si>
-  <si>
-    <t>Pivot by CC</t>
-  </si>
-  <si>
-    <t>VodafoneWorkingsRange</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -359,6 +335,21 @@
   </si>
   <si>
     <t>Monthly User Fee,VAT Reporting,Cash IQ,Casual User Scheme,DVLA Licence checks,Pay &amp; Reclaim,VISA 2 DRIVE</t>
+  </si>
+  <si>
+    <t>Inv</t>
+  </si>
+  <si>
+    <t>InvSheetName</t>
+  </si>
+  <si>
+    <t>InvRange</t>
+  </si>
+  <si>
+    <t>ActiveListReadRange</t>
+  </si>
+  <si>
+    <t>ActiveListSheetName</t>
   </si>
 </sst>
 </file>
@@ -748,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1008"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -801,7 +792,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -822,7 +813,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -841,31 +832,31 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -878,42 +869,42 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>77</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -921,20 +912,20 @@
         <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
@@ -942,145 +933,138 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>88</v>
-      </c>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" s="2"/>
+      <c r="A25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" s="2"/>
+      <c r="A28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="2" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44" t="s">
-        <v>106</v>
-      </c>
-    </row>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2044,7 +2028,6 @@
     <row r="1005" ht="14.25" customHeight="1"/>
     <row r="1006" ht="14.25" customHeight="1"/>
     <row r="1007" ht="14.25" customHeight="1"/>
-    <row r="1008" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3269,34 +3252,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
update performer after changes from uat
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Recharges_Performer_TMC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F46644-6C90-41A7-8810-07D6CB2F88F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0095B31E-672E-40BD-BC61-27C9EE0D10B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -319,9 +319,6 @@
     <t>HeaderSheetName</t>
   </si>
   <si>
-    <t>TMCRchges P{0}ACT</t>
-  </si>
-  <si>
     <t>FiscalText</t>
   </si>
   <si>
@@ -359,6 +356,159 @@
   </si>
   <si>
     <t>vbaExcludeSpecificValueInPivot</t>
+  </si>
+  <si>
+    <t>SetPivotTableRange</t>
+  </si>
+  <si>
+    <t>vbaSetPivotTableRange</t>
+  </si>
+  <si>
+    <t>SAP Dnl+Invoices</t>
+  </si>
+  <si>
+    <t>SapDnlSheetName</t>
+  </si>
+  <si>
+    <t>SapDnlRangePeriod</t>
+  </si>
+  <si>
+    <t>SapDnlRangeInvNo</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>SapDnlRangeTotalNetAmount</t>
+  </si>
+  <si>
+    <t>SapDnlRangePeriodDate</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>SapDnlRangePostingDate</t>
+  </si>
+  <si>
+    <t>P{0} TMC {1} ACT</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>JournalTextHeaderRange</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
+  <si>
+    <t>PreparedByRange</t>
+  </si>
+  <si>
+    <t>H15</t>
+  </si>
+  <si>
+    <t>DatePreparedRange</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>FinancialYearRange</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>DocumentDateRange</t>
+  </si>
+  <si>
+    <t>PostingDateRange</t>
+  </si>
+  <si>
+    <t>B16</t>
+  </si>
+  <si>
+    <t>PostingPeriodRange</t>
+  </si>
+  <si>
+    <t>SapDnlRangeDocumentDate</t>
+  </si>
+  <si>
+    <t>H16</t>
+  </si>
+  <si>
+    <t>H17</t>
+  </si>
+  <si>
+    <t>DateAuthorizedRange</t>
+  </si>
+  <si>
+    <t>DatePostedRange</t>
+  </si>
+  <si>
+    <t>Recharges_SaveScreenshotLocation</t>
+  </si>
+  <si>
+    <t>SapDnlCaptureRange</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>InsertPicture</t>
+  </si>
+  <si>
+    <t>vbaInsertPicture</t>
+  </si>
+  <si>
+    <t>A1:Q</t>
+  </si>
+  <si>
+    <t>InvUpdatedRange</t>
+  </si>
+  <si>
+    <t>PivotTable2</t>
+  </si>
+  <si>
+    <t>PivotTable3</t>
+  </si>
+  <si>
+    <t>PivotTable2InvSheet</t>
+  </si>
+  <si>
+    <t>PivotTable3InvSheet</t>
+  </si>
+  <si>
+    <t>PivotTable1CCColumn</t>
+  </si>
+  <si>
+    <t>CostCentre</t>
+  </si>
+  <si>
+    <t>PivotTable2CCColumn</t>
+  </si>
+  <si>
+    <t>For journal</t>
+  </si>
+  <si>
+    <t>PreparedByName</t>
+  </si>
+  <si>
+    <t>Robot</t>
   </si>
 </sst>
 </file>
@@ -376,6 +526,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -748,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -801,7 +952,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -822,7 +973,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -900,7 +1051,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>92</v>
       </c>
@@ -908,7 +1059,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>84</v>
       </c>
@@ -916,7 +1067,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>90</v>
       </c>
@@ -924,204 +1075,392 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
         <v>95</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A46" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A50" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A54" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
+      <c r="B55" t="s">
         <v>97</v>
       </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" s="6" t="s">
+    </row>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A58" t="s">
         <v>61</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B58" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
+    <row r="59" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B59" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
+    <row r="60" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
         <v>66</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B60" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
+    <row r="61" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
         <v>77</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B61" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
+    <row r="62" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
         <v>87</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B62" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" t="s">
         <v>106</v>
       </c>
-      <c r="B40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="6" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A65" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A66" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A67" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
         <v>69</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B68" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
         <v>80</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="74" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -2049,10 +2388,39 @@
     <row r="1005" ht="14.25" customHeight="1"/>
     <row r="1006" ht="14.25" customHeight="1"/>
     <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
+    <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
+    <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
+    <row r="1016" ht="14.25" customHeight="1"/>
+    <row r="1017" ht="14.25" customHeight="1"/>
+    <row r="1018" ht="14.25" customHeight="1"/>
+    <row r="1019" ht="14.25" customHeight="1"/>
+    <row r="1020" ht="14.25" customHeight="1"/>
+    <row r="1021" ht="14.25" customHeight="1"/>
+    <row r="1022" ht="14.25" customHeight="1"/>
+    <row r="1023" ht="14.25" customHeight="1"/>
+    <row r="1024" ht="14.25" customHeight="1"/>
+    <row r="1025" ht="14.25" customHeight="1"/>
+    <row r="1026" ht="14.25" customHeight="1"/>
+    <row r="1027" ht="14.25" customHeight="1"/>
+    <row r="1028" ht="14.25" customHeight="1"/>
+    <row r="1029" ht="14.25" customHeight="1"/>
+    <row r="1030" ht="14.25" customHeight="1"/>
+    <row r="1031" ht="14.25" customHeight="1"/>
+    <row r="1032" ht="14.25" customHeight="1"/>
+    <row r="1033" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -3216,6 +3584,9 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -3224,7 +3595,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3281,7 +3652,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
@@ -3289,21 +3660,28 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
-      </c>
-      <c r="B4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4301,5 +4679,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to open the PDF and take the screenshot in browser
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Recharges_Performer_TMC\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Darius\PRC_Recharges_Performer_TMC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8420E2F-7FF5-4296-B3C9-34DD4B8890AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8A441E-8896-46AF-BC0F-2D73734ECD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1212" yWindow="1224" windowWidth="23040" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -505,12 +505,6 @@
     <t>Robot</t>
   </si>
   <si>
-    <t>adobeExe</t>
-  </si>
-  <si>
-    <t>AcroRd32.exe</t>
-  </si>
-  <si>
     <t>DeleteAllSheetsButOne</t>
   </si>
   <si>
@@ -521,6 +515,12 @@
   </si>
   <si>
     <t>Monthly user fee,VAT Reporting,Cash iQ,Casual User Scheme,DVLA Licence checks,Receipt Checking - Pay &amp; Reclaim,Visa to Drive</t>
+  </si>
+  <si>
+    <t>chromeExe</t>
+  </si>
+  <si>
+    <t>chrome.exe</t>
   </si>
 </sst>
 </file>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1435,10 +1435,10 @@
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1">
@@ -1453,7 +1453,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1">
@@ -1461,7 +1461,7 @@
         <v>79</v>
       </c>
       <c r="B70" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1">
@@ -1469,10 +1469,10 @@
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1">

</xml_diff>